<commit_message>
processing SRRs to GSM for mixed dataset
</commit_message>
<xml_diff>
--- a/modEncode_chromatinChipSeq/modEncode_chromatinChipSeq_mix.xlsx
+++ b/modEncode_chromatinChipSeq/modEncode_chromatinChipSeq_mix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/semple/Documents/MeisterLab/Datasets/ChIP_seq_data_GEO/modEncode_chromatinChipSeq/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8DB3623E-BE43-BF43-84AD-C4079783A4A0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FB23264-64F7-944E-94CE-608602C197F0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3180" yWindow="2000" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{B7B36EF6-DB10-4544-8F04-869664F1C0C2}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20063,1825 +20063,1825 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{088262DD-036C-5049-8CD9-0C3ABC77BBCD}">
-  <dimension ref="B1:J291"/>
+  <dimension ref="A1:I291"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>251</v>
       </c>
       <c r="D2" t="s">
+        <v>252</v>
+      </c>
+      <c r="E2" t="s">
+        <v>253</v>
+      </c>
+      <c r="F2" t="s">
+        <v>254</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H4" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H5" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H6" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H8" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H19" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" t="s">
         <v>251</v>
       </c>
-      <c r="E2" t="s">
-        <v>252</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="D20" t="s">
+        <v>261</v>
+      </c>
+      <c r="E20" t="s">
         <v>253</v>
       </c>
-      <c r="G2" t="s">
+      <c r="F20" t="s">
         <v>254</v>
       </c>
-      <c r="H2" t="s">
+      <c r="G20" t="s">
         <v>15</v>
       </c>
-      <c r="I2" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I4" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I5" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I6" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I7" t="s">
+      <c r="H20" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D21" t="s">
+        <v>34</v>
+      </c>
+      <c r="H21" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H22" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H23" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H24" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I8" t="s">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H25" t="s">
         <v>22</v>
       </c>
-      <c r="J8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="J9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I10" t="s">
+      <c r="I25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H27" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H28" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H29" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H32" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>44</v>
+      </c>
+      <c r="B33" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33" t="s">
+        <v>251</v>
+      </c>
+      <c r="D33" t="s">
+        <v>267</v>
+      </c>
+      <c r="E33" t="s">
+        <v>253</v>
+      </c>
+      <c r="F33" t="s">
+        <v>254</v>
+      </c>
+      <c r="G33" t="s">
+        <v>15</v>
+      </c>
+      <c r="H33" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H34" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H35" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H36" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H37" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H38" t="s">
+        <v>22</v>
+      </c>
+      <c r="I38" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H39" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I11" t="s">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H40" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H41" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H42" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H45" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>55</v>
+      </c>
+      <c r="B46" t="s">
+        <v>56</v>
+      </c>
+      <c r="C46" t="s">
+        <v>272</v>
+      </c>
+      <c r="D46" t="s">
+        <v>267</v>
+      </c>
+      <c r="E46" t="s">
+        <v>253</v>
+      </c>
+      <c r="F46" t="s">
+        <v>254</v>
+      </c>
+      <c r="G46" t="s">
+        <v>15</v>
+      </c>
+      <c r="H46" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H47" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H48" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H49" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H50" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H51" t="s">
+        <v>22</v>
+      </c>
+      <c r="I51" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H52" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H53" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H56" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>65</v>
+      </c>
+      <c r="B57" t="s">
+        <v>66</v>
+      </c>
+      <c r="C57" t="s">
+        <v>251</v>
+      </c>
+      <c r="D57" t="s">
+        <v>277</v>
+      </c>
+      <c r="E57" t="s">
+        <v>253</v>
+      </c>
+      <c r="F57" t="s">
+        <v>254</v>
+      </c>
+      <c r="G57" t="s">
+        <v>15</v>
+      </c>
+      <c r="H57" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H58" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H59" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H60" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H61" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H62" t="s">
+        <v>22</v>
+      </c>
+      <c r="I62" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H63" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H64" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H65" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H66" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H69" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>75</v>
+      </c>
+      <c r="B70" t="s">
+        <v>76</v>
+      </c>
+      <c r="C70" t="s">
+        <v>272</v>
+      </c>
+      <c r="D70" t="s">
+        <v>277</v>
+      </c>
+      <c r="E70" t="s">
+        <v>253</v>
+      </c>
+      <c r="F70" t="s">
+        <v>254</v>
+      </c>
+      <c r="G70" t="s">
+        <v>15</v>
+      </c>
+      <c r="H70" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H71" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H72" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H73" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H74" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H75" t="s">
+        <v>22</v>
+      </c>
+      <c r="I75" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H76" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H77" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H80" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>83</v>
+      </c>
+      <c r="B81" t="s">
+        <v>84</v>
+      </c>
+      <c r="C81" t="s">
+        <v>251</v>
+      </c>
+      <c r="D81" t="s">
+        <v>286</v>
+      </c>
+      <c r="E81" t="s">
+        <v>253</v>
+      </c>
+      <c r="F81" t="s">
+        <v>254</v>
+      </c>
+      <c r="G81" t="s">
+        <v>15</v>
+      </c>
+      <c r="H81" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H82" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H83" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H84" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H85" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H86" t="s">
+        <v>22</v>
+      </c>
+      <c r="I86" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H87" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H88" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H89" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H90" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H93" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>93</v>
+      </c>
+      <c r="B94" t="s">
+        <v>94</v>
+      </c>
+      <c r="C94" t="s">
+        <v>272</v>
+      </c>
+      <c r="D94" t="s">
+        <v>286</v>
+      </c>
+      <c r="E94" t="s">
+        <v>253</v>
+      </c>
+      <c r="F94" t="s">
+        <v>254</v>
+      </c>
+      <c r="G94" t="s">
+        <v>15</v>
+      </c>
+      <c r="H94" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H95" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H96" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H97" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H98" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H99" t="s">
+        <v>22</v>
+      </c>
+      <c r="I99" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H100" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H101" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H104" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>101</v>
+      </c>
+      <c r="B105" t="s">
+        <v>102</v>
+      </c>
+      <c r="C105" t="s">
+        <v>251</v>
+      </c>
+      <c r="D105" t="s">
+        <v>295</v>
+      </c>
+      <c r="E105" t="s">
+        <v>253</v>
+      </c>
+      <c r="F105" t="s">
+        <v>254</v>
+      </c>
+      <c r="G105" t="s">
+        <v>15</v>
+      </c>
+      <c r="H105" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H106" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H107" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H108" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H109" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H110" t="s">
+        <v>22</v>
+      </c>
+      <c r="I110" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H111" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H112" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H113" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H114" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H117" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>111</v>
+      </c>
+      <c r="B118" t="s">
+        <v>112</v>
+      </c>
+      <c r="C118" t="s">
+        <v>272</v>
+      </c>
+      <c r="D118" t="s">
+        <v>295</v>
+      </c>
+      <c r="E118" t="s">
+        <v>253</v>
+      </c>
+      <c r="F118" t="s">
+        <v>254</v>
+      </c>
+      <c r="G118" t="s">
+        <v>15</v>
+      </c>
+      <c r="H118" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H119" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H120" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H121" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H122" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H123" t="s">
+        <v>22</v>
+      </c>
+      <c r="I123" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H124" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H125" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H128" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>118</v>
+      </c>
+      <c r="B129" t="s">
+        <v>119</v>
+      </c>
+      <c r="C129" t="s">
+        <v>251</v>
+      </c>
+      <c r="D129" t="s">
+        <v>304</v>
+      </c>
+      <c r="E129" t="s">
+        <v>253</v>
+      </c>
+      <c r="F129" t="s">
+        <v>254</v>
+      </c>
+      <c r="G129" t="s">
+        <v>15</v>
+      </c>
+      <c r="H129" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H130" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H131" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H132" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H133" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H134" t="s">
+        <v>22</v>
+      </c>
+      <c r="I134" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H135" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H136" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H137" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H138" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H141" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>128</v>
+      </c>
+      <c r="B142" t="s">
+        <v>129</v>
+      </c>
+      <c r="C142" t="s">
+        <v>272</v>
+      </c>
+      <c r="D142" t="s">
+        <v>304</v>
+      </c>
+      <c r="E142" t="s">
+        <v>253</v>
+      </c>
+      <c r="F142" t="s">
+        <v>254</v>
+      </c>
+      <c r="G142" t="s">
+        <v>15</v>
+      </c>
+      <c r="H142" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H143" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H144" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H145" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H146" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H147" t="s">
+        <v>22</v>
+      </c>
+      <c r="I147" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H148" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H149" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H152" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>135</v>
+      </c>
+      <c r="B153" t="s">
+        <v>136</v>
+      </c>
+      <c r="C153" t="s">
+        <v>251</v>
+      </c>
+      <c r="D153" t="s">
+        <v>313</v>
+      </c>
+      <c r="E153" t="s">
+        <v>253</v>
+      </c>
+      <c r="F153" t="s">
+        <v>254</v>
+      </c>
+      <c r="G153" t="s">
+        <v>15</v>
+      </c>
+      <c r="H153" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H154" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H155" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H156" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H157" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H158" t="s">
+        <v>22</v>
+      </c>
+      <c r="I158" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I159" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H160" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I12" t="s">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H161" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I13" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I19" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B20" t="s">
-        <v>31</v>
-      </c>
-      <c r="C20" t="s">
-        <v>32</v>
-      </c>
-      <c r="D20" t="s">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H162" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H163" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H166" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
+        <v>145</v>
+      </c>
+      <c r="B167" t="s">
+        <v>146</v>
+      </c>
+      <c r="C167" t="s">
         <v>251</v>
       </c>
-      <c r="E20" t="s">
-        <v>261</v>
-      </c>
-      <c r="F20" t="s">
+      <c r="D167" t="s">
+        <v>318</v>
+      </c>
+      <c r="E167" t="s">
         <v>253</v>
       </c>
-      <c r="G20" t="s">
+      <c r="F167" t="s">
         <v>254</v>
       </c>
-      <c r="H20" t="s">
+      <c r="G167" t="s">
         <v>15</v>
       </c>
-      <c r="I20" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="E21" t="s">
-        <v>34</v>
-      </c>
-      <c r="I21" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I22" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I23" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I24" t="s">
+      <c r="H167" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D168" t="s">
+        <v>148</v>
+      </c>
+      <c r="H168" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H169" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H170" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H171" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I25" t="s">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H172" t="s">
         <v>22</v>
       </c>
-      <c r="J25" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I26" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I27" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I28" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I29" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I32" t="s">
+      <c r="I172" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I173" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H174" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="175" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H175" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="176" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H176" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="177" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H177" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="180" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H180" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B33" t="s">
-        <v>44</v>
-      </c>
-      <c r="C33" t="s">
-        <v>45</v>
-      </c>
-      <c r="D33" t="s">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
+        <v>157</v>
+      </c>
+      <c r="B181" t="s">
+        <v>158</v>
+      </c>
+      <c r="C181" t="s">
         <v>251</v>
       </c>
-      <c r="E33" t="s">
-        <v>267</v>
-      </c>
-      <c r="F33" t="s">
+      <c r="D181" t="s">
+        <v>323</v>
+      </c>
+      <c r="E181" t="s">
         <v>253</v>
       </c>
-      <c r="G33" t="s">
+      <c r="F181" t="s">
         <v>254</v>
       </c>
-      <c r="H33" t="s">
+      <c r="G181" t="s">
         <v>15</v>
       </c>
-      <c r="I33" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I34" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I35" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I36" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I37" t="s">
+      <c r="H181" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="182" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H182" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="183" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H183" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="184" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H184" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="185" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H185" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I38" t="s">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H186" t="s">
         <v>22</v>
       </c>
-      <c r="J38" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I39" t="s">
+      <c r="I186" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="187" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I187" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="188" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H188" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="189" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H189" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="190" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H190" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="191" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H191" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="194" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H194" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="195" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A195" t="s">
+        <v>169</v>
+      </c>
+      <c r="B195" t="s">
+        <v>170</v>
+      </c>
+      <c r="C195" t="s">
+        <v>251</v>
+      </c>
+      <c r="D195" t="s">
+        <v>328</v>
+      </c>
+      <c r="E195" t="s">
+        <v>253</v>
+      </c>
+      <c r="F195" t="s">
+        <v>254</v>
+      </c>
+      <c r="G195" t="s">
+        <v>15</v>
+      </c>
+      <c r="H195" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="196" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H196" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="197" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H197" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="198" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H198" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="199" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H199" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="200" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H200" t="s">
+        <v>22</v>
+      </c>
+      <c r="I200" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="201" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H201" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I40" t="s">
+    <row r="202" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H202" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I41" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I42" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I45" t="s">
+    <row r="203" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H203" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="204" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H204" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="207" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H207" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B46" t="s">
-        <v>55</v>
-      </c>
-      <c r="C46" t="s">
-        <v>56</v>
-      </c>
-      <c r="D46" t="s">
+    <row r="208" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A208" t="s">
+        <v>179</v>
+      </c>
+      <c r="B208" t="s">
+        <v>180</v>
+      </c>
+      <c r="C208" t="s">
         <v>272</v>
       </c>
-      <c r="E46" t="s">
-        <v>267</v>
-      </c>
-      <c r="F46" t="s">
+      <c r="D208" t="s">
+        <v>328</v>
+      </c>
+      <c r="E208" t="s">
         <v>253</v>
       </c>
-      <c r="G46" t="s">
+      <c r="F208" t="s">
         <v>254</v>
       </c>
-      <c r="H46" t="s">
+      <c r="G208" t="s">
         <v>15</v>
       </c>
-      <c r="I46" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I47" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I48" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I49" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I50" t="s">
+      <c r="H208" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="209" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H209" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="210" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H210" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="211" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H211" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="212" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H212" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I51" t="s">
+    <row r="213" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H213" t="s">
         <v>22</v>
       </c>
-      <c r="J51" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I52" t="s">
+      <c r="I213" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="214" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H214" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="53" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I53" t="s">
+    <row r="215" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H215" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="56" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I56" t="s">
+    <row r="218" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H218" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="57" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B57" t="s">
-        <v>65</v>
-      </c>
-      <c r="C57" t="s">
-        <v>66</v>
-      </c>
-      <c r="D57" t="s">
+    <row r="219" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A219" t="s">
+        <v>186</v>
+      </c>
+      <c r="B219" t="s">
+        <v>187</v>
+      </c>
+      <c r="C219" t="s">
         <v>251</v>
       </c>
-      <c r="E57" t="s">
-        <v>277</v>
-      </c>
-      <c r="F57" t="s">
+      <c r="D219" t="s">
+        <v>337</v>
+      </c>
+      <c r="E219" t="s">
         <v>253</v>
       </c>
-      <c r="G57" t="s">
+      <c r="F219" t="s">
         <v>254</v>
       </c>
-      <c r="H57" t="s">
+      <c r="G219" t="s">
         <v>15</v>
       </c>
-      <c r="I57" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="58" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I58" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="59" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I59" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="60" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I60" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="61" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I61" t="s">
+      <c r="H219" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="220" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H220" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="221" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H221" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="222" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H222" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="223" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H223" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="62" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I62" t="s">
+    <row r="224" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H224" t="s">
         <v>22</v>
       </c>
-      <c r="J62" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="63" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I63" t="s">
+      <c r="I224" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="225" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H225" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="64" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I64" t="s">
+    <row r="226" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H226" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="65" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I65" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="66" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I66" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="69" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I69" t="s">
+    <row r="227" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H227" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="228" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H228" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="231" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H231" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="70" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B70" t="s">
-        <v>75</v>
-      </c>
-      <c r="C70" t="s">
-        <v>76</v>
-      </c>
-      <c r="D70" t="s">
+    <row r="232" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A232" t="s">
+        <v>196</v>
+      </c>
+      <c r="B232" t="s">
+        <v>197</v>
+      </c>
+      <c r="C232" t="s">
         <v>272</v>
       </c>
-      <c r="E70" t="s">
-        <v>277</v>
-      </c>
-      <c r="F70" t="s">
+      <c r="D232" t="s">
+        <v>337</v>
+      </c>
+      <c r="E232" t="s">
         <v>253</v>
       </c>
-      <c r="G70" t="s">
+      <c r="F232" t="s">
         <v>254</v>
       </c>
-      <c r="H70" t="s">
+      <c r="G232" t="s">
         <v>15</v>
       </c>
-      <c r="I70" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="71" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I71" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="72" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I72" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="73" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I73" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="74" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I74" t="s">
+      <c r="H232" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="233" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H233" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="234" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H234" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="235" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H235" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="236" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H236" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="75" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I75" t="s">
+    <row r="237" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H237" t="s">
         <v>22</v>
       </c>
-      <c r="J75" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="76" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I76" t="s">
+      <c r="I237" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="238" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H238" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="77" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I77" t="s">
+    <row r="239" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H239" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="80" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I80" t="s">
+    <row r="242" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H242" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="81" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B81" t="s">
-        <v>83</v>
-      </c>
-      <c r="C81" t="s">
-        <v>84</v>
-      </c>
-      <c r="D81" t="s">
+    <row r="243" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A243" t="s">
+        <v>203</v>
+      </c>
+      <c r="B243" t="s">
+        <v>204</v>
+      </c>
+      <c r="C243" t="s">
+        <v>346</v>
+      </c>
+      <c r="D243" t="s">
+        <v>347</v>
+      </c>
+      <c r="E243" t="s">
+        <v>253</v>
+      </c>
+      <c r="F243" t="s">
+        <v>254</v>
+      </c>
+      <c r="G243" t="s">
+        <v>15</v>
+      </c>
+      <c r="H243" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="244" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D244" t="s">
+        <v>207</v>
+      </c>
+      <c r="H244" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="245" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H245" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="246" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H246" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="247" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H247" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="248" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H248" t="s">
+        <v>22</v>
+      </c>
+      <c r="I248" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="249" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H249" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="250" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H250" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="251" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H251" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="254" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H254" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="255" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A255" t="s">
+        <v>217</v>
+      </c>
+      <c r="B255" t="s">
+        <v>218</v>
+      </c>
+      <c r="C255" t="s">
+        <v>346</v>
+      </c>
+      <c r="D255" t="s">
+        <v>353</v>
+      </c>
+      <c r="E255" t="s">
+        <v>253</v>
+      </c>
+      <c r="F255" t="s">
+        <v>254</v>
+      </c>
+      <c r="G255" t="s">
+        <v>15</v>
+      </c>
+      <c r="H255" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="256" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D256" t="s">
+        <v>220</v>
+      </c>
+      <c r="H256" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="257" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H257" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="258" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H258" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="259" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H259" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="260" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H260" t="s">
+        <v>22</v>
+      </c>
+      <c r="I260" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="261" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H261" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="262" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H262" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="263" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H263" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="266" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H266" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="267" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A267" t="s">
+        <v>228</v>
+      </c>
+      <c r="B267" t="s">
+        <v>229</v>
+      </c>
+      <c r="C267" t="s">
+        <v>346</v>
+      </c>
+      <c r="D267" t="s">
+        <v>358</v>
+      </c>
+      <c r="E267" t="s">
+        <v>253</v>
+      </c>
+      <c r="F267" t="s">
+        <v>254</v>
+      </c>
+      <c r="G267" t="s">
+        <v>15</v>
+      </c>
+      <c r="H267" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="268" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D268" t="s">
+        <v>231</v>
+      </c>
+      <c r="H268" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="269" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H269" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="270" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H270" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="271" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H271" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="272" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H272" t="s">
+        <v>22</v>
+      </c>
+      <c r="I272" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="273" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H273" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="274" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H274" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="275" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H275" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="278" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H278" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="279" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A279" t="s">
+        <v>239</v>
+      </c>
+      <c r="B279" t="s">
+        <v>240</v>
+      </c>
+      <c r="C279" t="s">
         <v>251</v>
       </c>
-      <c r="E81" t="s">
-        <v>286</v>
-      </c>
-      <c r="F81" t="s">
+      <c r="D279" t="s">
+        <v>363</v>
+      </c>
+      <c r="E279" t="s">
         <v>253</v>
       </c>
-      <c r="G81" t="s">
+      <c r="F279" t="s">
         <v>254</v>
       </c>
-      <c r="H81" t="s">
+      <c r="G279" t="s">
         <v>15</v>
       </c>
-      <c r="I81" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="82" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I82" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="83" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I83" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="84" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I84" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="85" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I85" t="s">
+      <c r="H279" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="280" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D280" t="s">
+        <v>242</v>
+      </c>
+      <c r="H280" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="281" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H281" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="282" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H282" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="283" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H283" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="86" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I86" t="s">
+    <row r="284" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H284" t="s">
         <v>22</v>
       </c>
-      <c r="J86" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="87" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I87" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="88" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I88" t="s">
+      <c r="I284" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="285" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H285" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="89" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I89" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="90" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I90" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="93" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I93" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="94" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B94" t="s">
-        <v>93</v>
-      </c>
-      <c r="C94" t="s">
-        <v>94</v>
-      </c>
-      <c r="D94" t="s">
-        <v>272</v>
-      </c>
-      <c r="E94" t="s">
-        <v>286</v>
-      </c>
-      <c r="F94" t="s">
-        <v>253</v>
-      </c>
-      <c r="G94" t="s">
-        <v>254</v>
-      </c>
-      <c r="H94" t="s">
-        <v>15</v>
-      </c>
-      <c r="I94" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="95" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I95" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="96" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I96" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="97" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I97" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="98" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I98" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="99" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I99" t="s">
-        <v>22</v>
-      </c>
-      <c r="J99" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="100" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I100" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="101" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I101" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="104" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I104" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="105" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B105" t="s">
-        <v>101</v>
-      </c>
-      <c r="C105" t="s">
-        <v>102</v>
-      </c>
-      <c r="D105" t="s">
-        <v>251</v>
-      </c>
-      <c r="E105" t="s">
-        <v>295</v>
-      </c>
-      <c r="F105" t="s">
-        <v>253</v>
-      </c>
-      <c r="G105" t="s">
-        <v>254</v>
-      </c>
-      <c r="H105" t="s">
-        <v>15</v>
-      </c>
-      <c r="I105" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="106" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I106" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="107" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I107" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="108" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I108" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="109" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I109" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="110" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I110" t="s">
-        <v>22</v>
-      </c>
-      <c r="J110" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="111" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I111" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="112" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I112" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="113" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I113" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="114" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I114" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="117" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I117" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="118" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B118" t="s">
-        <v>111</v>
-      </c>
-      <c r="C118" t="s">
-        <v>112</v>
-      </c>
-      <c r="D118" t="s">
-        <v>272</v>
-      </c>
-      <c r="E118" t="s">
-        <v>295</v>
-      </c>
-      <c r="F118" t="s">
-        <v>253</v>
-      </c>
-      <c r="G118" t="s">
-        <v>254</v>
-      </c>
-      <c r="H118" t="s">
-        <v>15</v>
-      </c>
-      <c r="I118" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="119" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I119" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="120" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I120" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="121" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I121" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="122" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I122" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="123" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I123" t="s">
-        <v>22</v>
-      </c>
-      <c r="J123" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="124" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I124" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="125" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I125" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="128" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I128" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="129" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B129" t="s">
-        <v>118</v>
-      </c>
-      <c r="C129" t="s">
-        <v>119</v>
-      </c>
-      <c r="D129" t="s">
-        <v>251</v>
-      </c>
-      <c r="E129" t="s">
-        <v>304</v>
-      </c>
-      <c r="F129" t="s">
-        <v>253</v>
-      </c>
-      <c r="G129" t="s">
-        <v>254</v>
-      </c>
-      <c r="H129" t="s">
-        <v>15</v>
-      </c>
-      <c r="I129" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="130" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I130" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="131" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I131" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="132" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I132" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="133" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I133" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="134" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I134" t="s">
-        <v>22</v>
-      </c>
-      <c r="J134" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="135" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I135" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="136" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I136" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="137" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I137" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="138" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I138" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="141" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I141" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="142" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B142" t="s">
-        <v>128</v>
-      </c>
-      <c r="C142" t="s">
-        <v>129</v>
-      </c>
-      <c r="D142" t="s">
-        <v>272</v>
-      </c>
-      <c r="E142" t="s">
-        <v>304</v>
-      </c>
-      <c r="F142" t="s">
-        <v>253</v>
-      </c>
-      <c r="G142" t="s">
-        <v>254</v>
-      </c>
-      <c r="H142" t="s">
-        <v>15</v>
-      </c>
-      <c r="I142" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="143" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I143" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="144" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I144" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="145" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I145" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="146" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I146" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="147" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I147" t="s">
-        <v>22</v>
-      </c>
-      <c r="J147" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="148" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I148" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="149" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I149" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="152" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I152" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="153" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B153" t="s">
-        <v>135</v>
-      </c>
-      <c r="C153" t="s">
-        <v>136</v>
-      </c>
-      <c r="D153" t="s">
-        <v>251</v>
-      </c>
-      <c r="E153" t="s">
-        <v>313</v>
-      </c>
-      <c r="F153" t="s">
-        <v>253</v>
-      </c>
-      <c r="G153" t="s">
-        <v>254</v>
-      </c>
-      <c r="H153" t="s">
-        <v>15</v>
-      </c>
-      <c r="I153" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="154" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I154" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="155" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I155" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="156" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I156" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="157" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I157" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="158" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I158" t="s">
-        <v>22</v>
-      </c>
-      <c r="J158" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="159" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="J159" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="160" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I160" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="161" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I161" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="162" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I162" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="163" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I163" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="166" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I166" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="167" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B167" t="s">
-        <v>145</v>
-      </c>
-      <c r="C167" t="s">
-        <v>146</v>
-      </c>
-      <c r="D167" t="s">
-        <v>251</v>
-      </c>
-      <c r="E167" t="s">
-        <v>318</v>
-      </c>
-      <c r="F167" t="s">
-        <v>253</v>
-      </c>
-      <c r="G167" t="s">
-        <v>254</v>
-      </c>
-      <c r="H167" t="s">
-        <v>15</v>
-      </c>
-      <c r="I167" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="168" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="E168" t="s">
-        <v>148</v>
-      </c>
-      <c r="I168" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="169" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I169" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="170" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I170" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="171" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I171" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="172" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I172" t="s">
-        <v>22</v>
-      </c>
-      <c r="J172" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="173" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="J173" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="174" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I174" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="175" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I175" t="s">
+    <row r="286" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H286" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="176" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I176" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="177" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I177" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="180" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I180" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="181" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B181" t="s">
-        <v>157</v>
-      </c>
-      <c r="C181" t="s">
-        <v>158</v>
-      </c>
-      <c r="D181" t="s">
-        <v>251</v>
-      </c>
-      <c r="E181" t="s">
-        <v>323</v>
-      </c>
-      <c r="F181" t="s">
-        <v>253</v>
-      </c>
-      <c r="G181" t="s">
-        <v>254</v>
-      </c>
-      <c r="H181" t="s">
-        <v>15</v>
-      </c>
-      <c r="I181" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="182" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I182" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="183" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I183" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="184" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I184" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="185" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I185" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="186" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I186" t="s">
-        <v>22</v>
-      </c>
-      <c r="J186" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="187" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="J187" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="188" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I188" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="189" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I189" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="190" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I190" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="191" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I191" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="194" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I194" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="195" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B195" t="s">
-        <v>169</v>
-      </c>
-      <c r="C195" t="s">
-        <v>170</v>
-      </c>
-      <c r="D195" t="s">
-        <v>251</v>
-      </c>
-      <c r="E195" t="s">
-        <v>328</v>
-      </c>
-      <c r="F195" t="s">
-        <v>253</v>
-      </c>
-      <c r="G195" t="s">
-        <v>254</v>
-      </c>
-      <c r="H195" t="s">
-        <v>15</v>
-      </c>
-      <c r="I195" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="196" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I196" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="197" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I197" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="198" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I198" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="199" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I199" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="200" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I200" t="s">
-        <v>22</v>
-      </c>
-      <c r="J200" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="201" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I201" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="202" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I202" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="203" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I203" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="204" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I204" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="207" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I207" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="208" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B208" t="s">
-        <v>179</v>
-      </c>
-      <c r="C208" t="s">
-        <v>180</v>
-      </c>
-      <c r="D208" t="s">
-        <v>272</v>
-      </c>
-      <c r="E208" t="s">
-        <v>328</v>
-      </c>
-      <c r="F208" t="s">
-        <v>253</v>
-      </c>
-      <c r="G208" t="s">
-        <v>254</v>
-      </c>
-      <c r="H208" t="s">
-        <v>15</v>
-      </c>
-      <c r="I208" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="209" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I209" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="210" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I210" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="211" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I211" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="212" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I212" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="213" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I213" t="s">
-        <v>22</v>
-      </c>
-      <c r="J213" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="214" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I214" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="215" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I215" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="218" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I218" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="219" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B219" t="s">
-        <v>186</v>
-      </c>
-      <c r="C219" t="s">
-        <v>187</v>
-      </c>
-      <c r="D219" t="s">
-        <v>251</v>
-      </c>
-      <c r="E219" t="s">
-        <v>337</v>
-      </c>
-      <c r="F219" t="s">
-        <v>253</v>
-      </c>
-      <c r="G219" t="s">
-        <v>254</v>
-      </c>
-      <c r="H219" t="s">
-        <v>15</v>
-      </c>
-      <c r="I219" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="220" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I220" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="221" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I221" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="222" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I222" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="223" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I223" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="224" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I224" t="s">
-        <v>22</v>
-      </c>
-      <c r="J224" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="225" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I225" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="226" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I226" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="227" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I227" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="228" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I228" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="231" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I231" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="232" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B232" t="s">
-        <v>196</v>
-      </c>
-      <c r="C232" t="s">
-        <v>197</v>
-      </c>
-      <c r="D232" t="s">
-        <v>272</v>
-      </c>
-      <c r="E232" t="s">
-        <v>337</v>
-      </c>
-      <c r="F232" t="s">
-        <v>253</v>
-      </c>
-      <c r="G232" t="s">
-        <v>254</v>
-      </c>
-      <c r="H232" t="s">
-        <v>15</v>
-      </c>
-      <c r="I232" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="233" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I233" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="234" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I234" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="235" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I235" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="236" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I236" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="237" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I237" t="s">
-        <v>22</v>
-      </c>
-      <c r="J237" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="238" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I238" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="239" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I239" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="242" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I242" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="243" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B243" t="s">
-        <v>203</v>
-      </c>
-      <c r="C243" t="s">
-        <v>204</v>
-      </c>
-      <c r="D243" t="s">
-        <v>346</v>
-      </c>
-      <c r="E243" t="s">
-        <v>347</v>
-      </c>
-      <c r="F243" t="s">
-        <v>253</v>
-      </c>
-      <c r="G243" t="s">
-        <v>254</v>
-      </c>
-      <c r="H243" t="s">
-        <v>15</v>
-      </c>
-      <c r="I243" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="244" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="E244" t="s">
-        <v>207</v>
-      </c>
-      <c r="I244" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="245" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I245" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="246" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I246" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="247" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I247" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="248" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I248" t="s">
-        <v>22</v>
-      </c>
-      <c r="J248" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="249" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I249" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="250" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I250" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="251" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I251" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="254" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I254" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="255" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B255" t="s">
-        <v>217</v>
-      </c>
-      <c r="C255" t="s">
-        <v>218</v>
-      </c>
-      <c r="D255" t="s">
-        <v>346</v>
-      </c>
-      <c r="E255" t="s">
-        <v>353</v>
-      </c>
-      <c r="F255" t="s">
-        <v>253</v>
-      </c>
-      <c r="G255" t="s">
-        <v>254</v>
-      </c>
-      <c r="H255" t="s">
-        <v>15</v>
-      </c>
-      <c r="I255" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="256" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="E256" t="s">
-        <v>220</v>
-      </c>
-      <c r="I256" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="257" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I257" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="258" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I258" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="259" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I259" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="260" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I260" t="s">
-        <v>22</v>
-      </c>
-      <c r="J260" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="261" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I261" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="262" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I262" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="263" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I263" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="266" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I266" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="267" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B267" t="s">
-        <v>228</v>
-      </c>
-      <c r="C267" t="s">
-        <v>229</v>
-      </c>
-      <c r="D267" t="s">
-        <v>346</v>
-      </c>
-      <c r="E267" t="s">
-        <v>358</v>
-      </c>
-      <c r="F267" t="s">
-        <v>253</v>
-      </c>
-      <c r="G267" t="s">
-        <v>254</v>
-      </c>
-      <c r="H267" t="s">
-        <v>15</v>
-      </c>
-      <c r="I267" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="268" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="E268" t="s">
-        <v>231</v>
-      </c>
-      <c r="I268" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="269" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I269" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="270" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I270" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="271" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I271" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="272" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I272" t="s">
-        <v>22</v>
-      </c>
-      <c r="J272" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="273" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I273" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="274" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I274" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="275" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I275" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="278" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I278" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="279" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B279" t="s">
-        <v>239</v>
-      </c>
-      <c r="C279" t="s">
-        <v>240</v>
-      </c>
-      <c r="D279" t="s">
-        <v>251</v>
-      </c>
-      <c r="E279" t="s">
-        <v>363</v>
-      </c>
-      <c r="F279" t="s">
-        <v>253</v>
-      </c>
-      <c r="G279" t="s">
-        <v>254</v>
-      </c>
-      <c r="H279" t="s">
-        <v>15</v>
-      </c>
-      <c r="I279" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="280" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="E280" t="s">
-        <v>242</v>
-      </c>
-      <c r="I280" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="281" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I281" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="282" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I282" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="283" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I283" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="284" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I284" t="s">
-        <v>22</v>
-      </c>
-      <c r="J284" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="285" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I285" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="286" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I286" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="287" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I287" t="s">
+    <row r="287" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H287" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="288" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="I288" t="s">
+    <row r="288" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H288" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="291" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I291" t="s">
+    <row r="291" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H291" t="s">
         <v>266</v>
       </c>
     </row>

</xml_diff>